<commit_message>
Fixed data set ranges and data frames
</commit_message>
<xml_diff>
--- a/Resources/real_hourly_compensation.xlsx
+++ b/Resources/real_hourly_compensation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trentonjpaxton/ClassFiles/class_project/class_project_1-/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trentonjpaxton/ClassFiles/class_project/class_project_1-/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0044F26C-8088-5E4A-888A-4786DBF8387F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3EB5D67-CB99-4047-ACAB-690C26593715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -82,20 +82,17 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -180,7 +177,7 @@
         <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A35F7E-B838-C830-243E-1B23C4D3BFAE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A44389A-D036-2627-E260-DFFEB9123D78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -531,11 +528,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -563,97 +560,114 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B2" s="3">
-        <v>8.8000000000000007</v>
+        <v>-0.8</v>
       </c>
       <c r="C2" s="3">
-        <v>-2.7</v>
+        <v>-0.1</v>
       </c>
       <c r="D2" s="3">
-        <v>-1.1000000000000001</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E2" s="3">
-        <v>4.0999999999999996</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B3" s="3">
-        <v>9.1999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C3" s="3">
-        <v>28.8</v>
+        <v>-2.7</v>
       </c>
       <c r="D3" s="3">
-        <v>-10.5</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="E3" s="3">
-        <v>7.5</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B4" s="3">
-        <v>-3.6</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C4" s="3">
-        <v>-1.7</v>
+        <v>28.8</v>
       </c>
       <c r="D4" s="3">
-        <v>-1</v>
+        <v>-10.5</v>
       </c>
       <c r="E4" s="3">
-        <v>-2.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B5" s="3">
-        <v>-6.6</v>
+        <v>-3.6</v>
       </c>
       <c r="C5" s="3">
-        <v>-8.5</v>
+        <v>-1.7</v>
       </c>
       <c r="D5" s="3">
-        <v>1.7</v>
+        <v>-1</v>
       </c>
       <c r="E5" s="3">
-        <v>-3.9</v>
+        <v>-2.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B6" s="3">
-        <v>2.9</v>
+        <v>-6.6</v>
       </c>
       <c r="C6" s="3">
-        <v>2.8</v>
+        <v>-8.5</v>
       </c>
       <c r="D6" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.7</v>
       </c>
       <c r="E6" s="3">
-        <v>-2</v>
+        <v>-3.9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>2024</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="3">
         <v>0.4</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C8" s="3">
         <v>0.1</v>
       </c>
     </row>
@@ -662,7 +676,7 @@
   <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddHeader>&amp;CBureau of Labor Statistics</oddHeader>
-    <oddFooter>&amp;LSource: Bureau of Labor Statistics&amp;RGenerated on: November 4, 2024 (11:15:43 PM)</oddFooter>
+    <oddFooter>&amp;LSource: Bureau of Labor Statistics&amp;RGenerated on: November 5, 2024 (12:53:05 AM)</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>